<commit_message>
[TimesheetCalculatorV2] Changes: * implemented the calculation of totals hours * added calculator tests * initialized model in main.py * renamed start_time and end_time to time_in and time_out respectively. * added timesheet progress dialog, so that users know the progress during generation of results. * implemented timesheet model * added extra condition in timesheet_parser.py to check if its the correct excel file. * added test data
</commit_message>
<xml_diff>
--- a/python_source/Timesheet_Calculator_v2/test/parser/testdata/timesheet_parser_testdata_001.xlsx
+++ b/python_source/Timesheet_Calculator_v2/test/parser/testdata/timesheet_parser_testdata_001.xlsx
@@ -9,6 +9,7 @@
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="secret_identifier" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -101,11 +102,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/mmm/yyyy"/>
     <numFmt numFmtId="166" formatCode="hh:mm\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="d/mmm/yyyy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -240,7 +240,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -290,10 +290,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,7 +380,7 @@
       <selection pane="topLeft" activeCell="J35" activeCellId="0" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.83"/>
@@ -551,7 +547,7 @@
       <c r="G24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E25" s="14"/>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
@@ -586,4 +582,27 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>